<commit_message>
changed run bat file
</commit_message>
<xml_diff>
--- a/Mongo_Search/Config.xlsx
+++ b/Mongo_Search/Config.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaayem\Documents\Python\Kym\Mongo_Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AE7C6D-FCEF-43C1-9754-3D4A0243A744}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27539D46-59D2-437F-B211-C6D70EB8BEF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{50ED4C38-B0C0-4F98-BDF2-F7ADD0C76675}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{50ED4C38-B0C0-4F98-BDF2-F7ADD0C76675}"/>
   </bookViews>
   <sheets>
     <sheet name="GSR" sheetId="1" r:id="rId1"/>
     <sheet name="MMsearch" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Search functions" sheetId="4" r:id="rId3"/>
     <sheet name="MMcheck" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>code</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Metrics</t>
-  </si>
-  <si>
     <t>AE</t>
   </si>
   <si>
@@ -85,6 +82,12 @@
   </si>
   <si>
     <t>channel</t>
+  </si>
+  <si>
+    <t>Average Stock Units</t>
+  </si>
+  <si>
+    <t>metric</t>
   </si>
 </sst>
 </file>
@@ -453,14 +456,14 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -472,36 +475,36 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="E2" t="s">
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -514,39 +517,39 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>